<commit_message>
sundar bast estimate corrected to send to milan sir for checking
</commit_message>
<xml_diff>
--- a/ofc/estimates/सुन्दर बस्ती सडक/सुन्दर बस्ती सडक.xlsx
+++ b/ofc/estimates/सुन्दर बस्ती सडक/सुन्दर बस्ती सडक.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Videos\079-080\samjhauta huna baki\सुन्दर बस्ती सडक\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\सुन्दर बस्ती सडक\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estimate" sheetId="4" state="hidden" r:id="rId1"/>
@@ -21,6 +21,7 @@
   <externalReferences>
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="description_103">[1]Abstract!$B$16</definedName>
@@ -31,11 +32,13 @@
     <definedName name="description_261">[2]Abstract!$B$33</definedName>
     <definedName name="description_262">[1]Abstract!$B$34</definedName>
     <definedName name="description_3">[1]Abstract!$B$169</definedName>
+    <definedName name="description_310">[3]Abstract!$B$60</definedName>
     <definedName name="description_5">[1]Abstract!$B$171</definedName>
+    <definedName name="description_6">[3]Abstract!$B$172</definedName>
     <definedName name="description_759">[1]Abstract!$B$278</definedName>
     <definedName name="description_783">[1]Abstract!$B$301</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Estimate!$A$1:$K$78</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">final!$A$1:$K$54</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">final!$A$1:$K$60</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">measurement!$A$1:$K$22</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">Valuated!$A$1:$K$22</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Estimate!$1:$8</definedName>
@@ -62,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="85">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -298,21 +301,37 @@
     <t>-450mm dia hume pipe</t>
   </si>
   <si>
-    <t>Providing and laying Brick Masonry Work in Cement mortar  in Foundation / structure complete excluding Pointing and Plastering, as per Drawing and Technical Specifications., Cement sand mortar (1:6)</t>
-  </si>
-  <si>
     <t>-Deduction for opening</t>
+  </si>
+  <si>
+    <t>Providing and Laying Reinforced cement concrete NP3 Flush jointed pipe for culverts including fixing with cement mortar 1:2 as per Drawing and Technical Specifications., 600 mm  internal dia.</t>
+  </si>
+  <si>
+    <t>Providing and laying of hand pack Stone soling with 150 to 200 mm thick stones and packing with smaller stone on prepared surface as per Drawing and Technical Specifications.</t>
+  </si>
+  <si>
+    <t>Providing and laying of Plain/Reinforced Cement Concrete in Foundation complete as per Drawing and Technical Specifications., RCC Grade M 20</t>
+  </si>
+  <si>
+    <t>Length (m)</t>
+  </si>
+  <si>
+    <t>Unit weight (kg/m)</t>
+  </si>
+  <si>
+    <t>e'O{+tNnfdf lrDgL e§fsf] O{+6fsf] uf/f] l;d]G6 d;nf -!M^_ df</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,8 +444,12 @@
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Preeti"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -436,6 +459,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,9 +530,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -511,7 +540,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -522,7 +551,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -535,7 +564,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -551,7 +580,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -560,7 +589,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -572,7 +601,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -597,7 +626,7 @@
     <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -624,7 +653,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
@@ -635,7 +664,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -671,40 +700,55 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -726,23 +770,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -788,8 +833,8 @@
       <sheetName val="PPMO_BOQ"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1">
         <row r="16">
           <cell r="B16" t="str">
             <v>Clearing and Grubbing Road Land ., Clearing and grubbing road land including uprooting rank vegetation, grass, bushes, shrubs, saplings and trees girth up to 300 mm, removal of stumps of trees cut earlier and disposal of unserviceable materials and stacking of serviceable Material to be used or auctioned, up to a lead of 30 meters including removal and disposal of top organic soil not exceeding 150 mm in thickness., By Mechanical Means, In area of light jungle (less than 15 number per 100 sqm )</v>
@@ -831,25 +876,25 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -882,11 +927,75 @@
       <sheetName val="PPMO_BOQ"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1">
         <row r="33">
           <cell r="B33" t="str">
             <v>Earthwork Excavation in Cutting., Roadway Excavation in all types of Soil by Manual Means ., Roadway Excavation in all types of soil as per drawing and technical specification, including removal of stumps and other deleterious matter, with all lifts and lead as per Drawing and instruction of the Engineer.</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Datasheet"/>
+      <sheetName val="Abstract"/>
+      <sheetName val="Quantity_Sheet"/>
+      <sheetName val="District_Rate"/>
+      <sheetName val="Equipment_Rate"/>
+      <sheetName val="Summary_of_Rates"/>
+      <sheetName val="rate (roadway)"/>
+      <sheetName val="manhole"/>
+      <sheetName val="bistar"/>
+      <sheetName val="Rate_Analysis"/>
+      <sheetName val="DWC pipe Rate-analysis"/>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Sheet3"/>
+      <sheetName val="Sheet4"/>
+      <sheetName val="Loading_Unloading"/>
+      <sheetName val="Collection"/>
+      <sheetName val="Transportation"/>
+      <sheetName val="References"/>
+      <sheetName val="BOQ"/>
+      <sheetName val="PPMO_BOQ"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="60">
+          <cell r="B60" t="str">
+            <v>Providing and laying of hand pack Stone soling with 150 to 200 mm thick stones and packing with smaller stone on prepared surface as per Drawing and Technical Specifications.</v>
+          </cell>
+        </row>
+        <row r="172">
+          <cell r="B172" t="str">
+            <v>Providing and laying of Plain/Reinforced Cement Concrete in Foundation complete as per Drawing and Technical Specifications., RCC Grade M 20</v>
           </cell>
         </row>
       </sheetData>
@@ -1183,26 +1292,26 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="7" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" customWidth="1"/>
+    <col min="14" max="14" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" customWidth="1"/>
+    <col min="17" max="17" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
@@ -1217,7 +1326,7 @@
       <c r="J1" s="74"/>
       <c r="K1" s="74"/>
     </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A2" s="75" t="s">
         <v>1</v>
       </c>
@@ -1232,7 +1341,7 @@
       <c r="J2" s="75"/>
       <c r="K2" s="75"/>
     </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="76" t="s">
         <v>2</v>
       </c>
@@ -1247,7 +1356,7 @@
       <c r="J3" s="76"/>
       <c r="K3" s="76"/>
     </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="76" t="s">
         <v>3</v>
       </c>
@@ -1262,7 +1371,7 @@
       <c r="J4" s="76"/>
       <c r="K4" s="76"/>
     </row>
-    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="77" t="s">
         <v>4</v>
       </c>
@@ -1277,41 +1386,41 @@
       <c r="J5" s="77"/>
       <c r="K5" s="77"/>
     </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="78" t="s">
+    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="79" t="s">
+      <c r="H6" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="80" t="s">
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="79" t="s">
+      <c r="H7" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1346,7 +1455,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="156" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>1</v>
       </c>
@@ -1371,7 +1480,7 @@
       <c r="R9" s="36"/>
       <c r="S9" s="36"/>
     </row>
-    <row r="10" spans="1:19" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A10" s="29"/>
       <c r="B10" s="61" t="s">
         <v>62</v>
@@ -1405,7 +1514,7 @@
       <c r="R10" s="36"/>
       <c r="S10" s="36"/>
     </row>
-    <row r="11" spans="1:19" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A11" s="29"/>
       <c r="B11" s="61" t="s">
         <v>60</v>
@@ -1441,7 +1550,7 @@
       <c r="R11" s="36"/>
       <c r="S11" s="36"/>
     </row>
-    <row r="12" spans="1:19" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A12" s="29"/>
       <c r="B12" s="61" t="s">
         <v>64</v>
@@ -1480,7 +1589,7 @@
       <c r="R12" s="36"/>
       <c r="S12" s="36"/>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29"/>
       <c r="B13" s="60" t="s">
         <v>58</v>
@@ -1512,7 +1621,7 @@
       <c r="R13" s="36"/>
       <c r="S13" s="36"/>
     </row>
-    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29"/>
       <c r="B14" s="60" t="s">
         <v>51</v>
@@ -1537,7 +1646,7 @@
       <c r="R14" s="36"/>
       <c r="S14" s="36"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29"/>
       <c r="B15" s="35"/>
       <c r="C15" s="30"/>
@@ -1557,7 +1666,7 @@
       <c r="R15" s="36"/>
       <c r="S15" s="36"/>
     </row>
-    <row r="16" spans="1:19" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
         <v>2</v>
       </c>
@@ -1574,7 +1683,7 @@
       <c r="J16" s="50"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="61" t="s">
         <v>62</v>
@@ -1602,7 +1711,7 @@
       <c r="J17" s="50"/>
       <c r="K17" s="5"/>
     </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="61" t="s">
         <v>60</v>
@@ -1631,7 +1740,7 @@
       <c r="J18" s="50"/>
       <c r="K18" s="5"/>
     </row>
-    <row r="19" spans="1:19" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A19" s="29"/>
       <c r="B19" s="61" t="s">
         <v>64</v>
@@ -1667,7 +1776,7 @@
       <c r="R19" s="36"/>
       <c r="S19" s="36"/>
     </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" s="60" t="s">
         <v>58</v>
@@ -1692,7 +1801,7 @@
       </c>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
       <c r="B21" s="60" t="s">
         <v>51</v>
@@ -1710,7 +1819,7 @@
       </c>
       <c r="K21" s="5"/>
     </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29"/>
       <c r="B22" s="35"/>
       <c r="C22" s="30"/>
@@ -1730,7 +1839,7 @@
       <c r="R22" s="36"/>
       <c r="S22" s="36"/>
     </row>
-    <row r="23" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="69" x14ac:dyDescent="0.3">
       <c r="A23" s="29">
         <v>3</v>
       </c>
@@ -1754,7 +1863,7 @@
       <c r="R23" s="36"/>
       <c r="S23" s="36"/>
     </row>
-    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
       <c r="B24" s="61" t="s">
         <v>64</v>
@@ -1782,7 +1891,7 @@
       <c r="J24" s="50"/>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" s="61" t="s">
         <v>65</v>
@@ -1809,7 +1918,7 @@
       <c r="J25" s="50"/>
       <c r="K25" s="5"/>
     </row>
-    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
       <c r="B26" s="61" t="s">
         <v>60</v>
@@ -1838,7 +1947,7 @@
       <c r="J26" s="50"/>
       <c r="K26" s="5"/>
     </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
       <c r="B27" s="60" t="s">
         <v>58</v>
@@ -1863,7 +1972,7 @@
       </c>
       <c r="K27" s="5"/>
     </row>
-    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
       <c r="B28" s="60" t="s">
         <v>51</v>
@@ -1881,7 +1990,7 @@
       </c>
       <c r="K28" s="5"/>
     </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="29"/>
       <c r="B29" s="35"/>
       <c r="C29" s="30"/>
@@ -1901,7 +2010,7 @@
       <c r="R29" s="36"/>
       <c r="S29" s="36"/>
     </row>
-    <row r="30" spans="1:19" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A30" s="29">
         <v>4</v>
       </c>
@@ -1926,7 +2035,7 @@
       <c r="R30" s="36"/>
       <c r="S30" s="36"/>
     </row>
-    <row r="31" spans="1:19" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A31" s="29"/>
       <c r="B31" s="62" t="s">
         <v>60</v>
@@ -1961,7 +2070,7 @@
       <c r="R31" s="36"/>
       <c r="S31" s="36"/>
     </row>
-    <row r="32" spans="1:19" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A32" s="29"/>
       <c r="B32" s="62" t="s">
         <v>61</v>
@@ -1995,7 +2104,7 @@
       <c r="R32" s="36"/>
       <c r="S32" s="36"/>
     </row>
-    <row r="33" spans="1:19" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A33" s="29"/>
       <c r="B33" s="60" t="s">
         <v>58</v>
@@ -2027,7 +2136,7 @@
       <c r="R33" s="36"/>
       <c r="S33" s="36"/>
     </row>
-    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="29"/>
       <c r="B34" s="60" t="s">
         <v>51</v>
@@ -2052,7 +2161,7 @@
       <c r="R34" s="36"/>
       <c r="S34" s="36"/>
     </row>
-    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="29"/>
       <c r="B35" s="60"/>
       <c r="C35" s="5"/>
@@ -2072,7 +2181,7 @@
       <c r="R35" s="36"/>
       <c r="S35" s="36"/>
     </row>
-    <row r="36" spans="1:19" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A36" s="29">
         <v>5</v>
       </c>
@@ -2097,7 +2206,7 @@
       <c r="R36" s="36"/>
       <c r="S36" s="36"/>
     </row>
-    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="29"/>
       <c r="B37" s="60" t="s">
         <v>64</v>
@@ -2131,7 +2240,7 @@
       <c r="R37" s="36"/>
       <c r="S37" s="36"/>
     </row>
-    <row r="38" spans="1:19" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A38" s="29"/>
       <c r="B38" s="60" t="s">
         <v>58</v>
@@ -2163,7 +2272,7 @@
       <c r="R38" s="36"/>
       <c r="S38" s="36"/>
     </row>
-    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="29"/>
       <c r="B39" s="60" t="s">
         <v>51</v>
@@ -2188,7 +2297,7 @@
       <c r="R39" s="36"/>
       <c r="S39" s="36"/>
     </row>
-    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="29"/>
       <c r="B40" s="60"/>
       <c r="C40" s="5"/>
@@ -2208,7 +2317,7 @@
       <c r="R40" s="36"/>
       <c r="S40" s="36"/>
     </row>
-    <row r="41" spans="1:19" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="78" x14ac:dyDescent="0.3">
       <c r="A41" s="29">
         <v>6</v>
       </c>
@@ -2233,7 +2342,7 @@
       <c r="R41" s="36"/>
       <c r="S41" s="36"/>
     </row>
-    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="29"/>
       <c r="B42" s="60" t="str">
         <f>B17</f>
@@ -2270,7 +2379,7 @@
       <c r="R42" s="36"/>
       <c r="S42" s="36"/>
     </row>
-    <row r="43" spans="1:19" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A43" s="29"/>
       <c r="B43" s="60" t="s">
         <v>58</v>
@@ -2302,7 +2411,7 @@
       <c r="R43" s="36"/>
       <c r="S43" s="36"/>
     </row>
-    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="29"/>
       <c r="B44" s="60" t="s">
         <v>51</v>
@@ -2327,7 +2436,7 @@
       <c r="R44" s="36"/>
       <c r="S44" s="36"/>
     </row>
-    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="29"/>
       <c r="B45" s="60"/>
       <c r="C45" s="5"/>
@@ -2347,7 +2456,7 @@
       <c r="R45" s="36"/>
       <c r="S45" s="36"/>
     </row>
-    <row r="46" spans="1:19" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="78" x14ac:dyDescent="0.3">
       <c r="A46" s="29">
         <v>7</v>
       </c>
@@ -2377,7 +2486,7 @@
       <c r="R46" s="36"/>
       <c r="S46" s="36"/>
     </row>
-    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="29"/>
       <c r="B47" s="62" t="s">
         <v>67</v>
@@ -2414,7 +2523,7 @@
       <c r="R47" s="36"/>
       <c r="S47" s="36"/>
     </row>
-    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="29"/>
       <c r="B48" s="62" t="s">
         <v>68</v>
@@ -2451,7 +2560,7 @@
       <c r="R48" s="36"/>
       <c r="S48" s="36"/>
     </row>
-    <row r="49" spans="1:19" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A49" s="29"/>
       <c r="B49" s="60" t="s">
         <v>58</v>
@@ -2483,7 +2592,7 @@
       <c r="R49" s="36"/>
       <c r="S49" s="36"/>
     </row>
-    <row r="50" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="29"/>
       <c r="B50" s="60" t="s">
         <v>51</v>
@@ -2508,7 +2617,7 @@
       <c r="R50" s="36"/>
       <c r="S50" s="36"/>
     </row>
-    <row r="51" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="29"/>
       <c r="B51" s="46"/>
       <c r="C51" s="30"/>
@@ -2528,7 +2637,7 @@
       <c r="R51" s="36"/>
       <c r="S51" s="36"/>
     </row>
-    <row r="52" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="11">
         <v>8</v>
       </c>
@@ -2545,7 +2654,7 @@
       <c r="J52" s="50"/>
       <c r="K52" s="5"/>
     </row>
-    <row r="53" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="11">
         <v>8.1</v>
       </c>
@@ -2562,7 +2671,7 @@
       <c r="J53" s="50"/>
       <c r="K53" s="5"/>
     </row>
-    <row r="54" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="11"/>
       <c r="B54" s="5" t="s">
         <v>55</v>
@@ -2589,7 +2698,7 @@
       <c r="J54" s="50"/>
       <c r="K54" s="5"/>
     </row>
-    <row r="55" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="11"/>
       <c r="B55" s="60" t="s">
         <v>58</v>
@@ -2614,7 +2723,7 @@
       </c>
       <c r="K55" s="5"/>
     </row>
-    <row r="56" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="11"/>
       <c r="B56" s="60" t="s">
         <v>51</v>
@@ -2632,7 +2741,7 @@
       </c>
       <c r="K56" s="5"/>
     </row>
-    <row r="57" spans="1:19" ht="105" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A57" s="11">
         <v>8.1999999999999993</v>
       </c>
@@ -2649,7 +2758,7 @@
       <c r="J57" s="50"/>
       <c r="K57" s="5"/>
     </row>
-    <row r="58" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="11"/>
       <c r="B58" s="5" t="s">
         <v>55</v>
@@ -2676,7 +2785,7 @@
       <c r="J58" s="50"/>
       <c r="K58" s="5"/>
     </row>
-    <row r="59" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="11"/>
       <c r="B59" s="60" t="s">
         <v>58</v>
@@ -2705,7 +2814,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="11"/>
       <c r="B60" s="60" t="s">
         <v>51</v>
@@ -2723,7 +2832,7 @@
       </c>
       <c r="K60" s="5"/>
     </row>
-    <row r="61" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="11"/>
       <c r="B61" s="5"/>
       <c r="C61" s="48"/>
@@ -2736,7 +2845,7 @@
       <c r="J61" s="56"/>
       <c r="K61" s="5"/>
     </row>
-    <row r="62" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="11">
         <v>8.3000000000000007</v>
       </c>
@@ -2753,7 +2862,7 @@
       <c r="J62" s="56"/>
       <c r="K62" s="18"/>
     </row>
-    <row r="63" spans="1:19" ht="105" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A63" s="11"/>
       <c r="B63" s="58" t="str">
         <f>description_247</f>
@@ -2777,7 +2886,7 @@
       <c r="J63" s="59"/>
       <c r="K63" s="18"/>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" s="11"/>
       <c r="B64" s="60" t="s">
         <v>58</v>
@@ -2802,7 +2911,7 @@
       </c>
       <c r="K64" s="18"/>
     </row>
-    <row r="65" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="11"/>
       <c r="B65" s="60" t="s">
         <v>51</v>
@@ -2820,7 +2929,7 @@
       </c>
       <c r="K65" s="19"/>
     </row>
-    <row r="66" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="29"/>
       <c r="B66" s="46"/>
       <c r="C66" s="30"/>
@@ -2840,7 +2949,7 @@
       <c r="R66" s="36"/>
       <c r="S66" s="36"/>
     </row>
-    <row r="67" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="29"/>
       <c r="B67" s="46"/>
       <c r="C67" s="30"/>
@@ -2860,7 +2969,7 @@
       <c r="R67" s="36"/>
       <c r="S67" s="36"/>
     </row>
-    <row r="68" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="29"/>
       <c r="B68" s="46"/>
       <c r="C68" s="30"/>
@@ -2880,7 +2989,7 @@
       <c r="R68" s="36"/>
       <c r="S68" s="36"/>
     </row>
-    <row r="69" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="29">
         <v>9</v>
       </c>
@@ -2916,7 +3025,7 @@
       <c r="R69" s="36"/>
       <c r="S69" s="36"/>
     </row>
-    <row r="70" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="29"/>
       <c r="B70" s="35"/>
       <c r="C70" s="30"/>
@@ -2936,7 +3045,7 @@
       <c r="R70" s="36"/>
       <c r="S70" s="36"/>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A71" s="11"/>
       <c r="B71" s="28" t="s">
         <v>17</v>
@@ -2954,15 +3063,15 @@
       </c>
       <c r="K71" s="5"/>
     </row>
-    <row r="73" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B73" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C73" s="70">
+      <c r="C73" s="72">
         <f>J71</f>
         <v>1194331.7948368895</v>
       </c>
-      <c r="D73" s="71"/>
+      <c r="D73" s="73"/>
       <c r="E73" s="16">
         <v>100</v>
       </c>
@@ -2973,87 +3082,87 @@
       <c r="J73" s="23"/>
       <c r="K73" s="24"/>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B74" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C74" s="72">
+      <c r="C74" s="79">
         <v>1000000</v>
       </c>
-      <c r="D74" s="73"/>
+      <c r="D74" s="80"/>
       <c r="E74" s="16"/>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B75" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C75" s="72">
+      <c r="C75" s="79">
         <f>C74-C77-C78</f>
         <v>950000</v>
       </c>
-      <c r="D75" s="73"/>
+      <c r="D75" s="80"/>
       <c r="E75" s="16">
         <f>C75/C73*100</f>
         <v>79.542385466656867</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B76" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C76" s="69">
+      <c r="C76" s="78">
         <f>C73-C75</f>
         <v>244331.79483688949</v>
       </c>
-      <c r="D76" s="69"/>
+      <c r="D76" s="78"/>
       <c r="E76" s="16">
         <f>100-E75</f>
         <v>20.457614533343133</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B77" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C77" s="70">
+      <c r="C77" s="72">
         <f>C74*0.03</f>
         <v>30000</v>
       </c>
-      <c r="D77" s="71"/>
+      <c r="D77" s="73"/>
       <c r="E77" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B78" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C78" s="70">
+      <c r="C78" s="72">
         <f>C74*0.02</f>
         <v>20000</v>
       </c>
-      <c r="D78" s="71"/>
+      <c r="D78" s="73"/>
       <c r="E78" s="16">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="A7:F7"/>
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="C73:D73"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3066,32 +3175,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S54"/>
+  <dimension ref="A1:S60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="N41" sqref="N41"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="7" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" customWidth="1"/>
+    <col min="14" max="14" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" customWidth="1"/>
+    <col min="17" max="17" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
@@ -3106,7 +3215,7 @@
       <c r="J1" s="74"/>
       <c r="K1" s="74"/>
     </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A2" s="75" t="s">
         <v>1</v>
       </c>
@@ -3121,7 +3230,7 @@
       <c r="J2" s="75"/>
       <c r="K2" s="75"/>
     </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="76" t="s">
         <v>2</v>
       </c>
@@ -3136,7 +3245,7 @@
       <c r="J3" s="76"/>
       <c r="K3" s="76"/>
     </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="76" t="s">
         <v>3</v>
       </c>
@@ -3151,7 +3260,7 @@
       <c r="J4" s="76"/>
       <c r="K4" s="76"/>
     </row>
-    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="77" t="s">
         <v>4</v>
       </c>
@@ -3166,41 +3275,41 @@
       <c r="J5" s="77"/>
       <c r="K5" s="77"/>
     </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="78" t="s">
+    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="79" t="s">
+      <c r="H6" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="80" t="s">
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="79" t="s">
+      <c r="H7" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -3235,7 +3344,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>1</v>
       </c>
@@ -3256,7 +3365,7 @@
       <c r="R9" s="68"/>
       <c r="S9" s="68"/>
     </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29"/>
       <c r="B10" s="60" t="s">
         <v>74</v>
@@ -3265,18 +3374,18 @@
         <v>1</v>
       </c>
       <c r="D10" s="8">
-        <f>7*2+3.5</f>
-        <v>17.5</v>
+        <f>20+24-4*1.2+20</f>
+        <v>59.2</v>
       </c>
       <c r="E10" s="8">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="F10" s="8">
-        <v>0.6</v>
+        <v>1.2</v>
       </c>
       <c r="G10" s="63">
-        <f t="shared" ref="G10:G11" si="0">PRODUCT(C10:F10)</f>
-        <v>6.3</v>
+        <f>PRODUCT(C10:F10)</f>
+        <v>53.280000000000008</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
@@ -3290,25 +3399,26 @@
       <c r="R10" s="36"/>
       <c r="S10" s="36"/>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29"/>
-      <c r="B11" s="61"/>
+      <c r="B11" s="60" t="s">
+        <v>60</v>
+      </c>
       <c r="C11" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D11" s="8">
-        <f>(3*7+2)+(6*7+5)+(4*7+2)-50</f>
-        <v>50</v>
+        <v>1.2</v>
       </c>
       <c r="E11" s="8">
-        <v>0.45</v>
+        <v>1.2</v>
       </c>
       <c r="F11" s="8">
-        <v>0.45</v>
+        <v>1.5</v>
       </c>
       <c r="G11" s="63">
-        <f t="shared" si="0"/>
-        <v>10.125</v>
+        <f>C11*(PI())*(D11*E11/4)*F11</f>
+        <v>8.4823001646924414</v>
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
@@ -3322,30 +3432,29 @@
       <c r="R11" s="36"/>
       <c r="S11" s="36"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29"/>
       <c r="B12" s="60" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="5">
-        <v>3</v>
-      </c>
-      <c r="D12" s="8">
-        <v>1</v>
-      </c>
-      <c r="E12" s="8">
-        <v>1</v>
-      </c>
-      <c r="F12" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="G12" s="63">
-        <f>C12*(PI())*(D12*E12/4)*F12</f>
-        <v>2.8274333882308138</v>
-      </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
+        <v>58</v>
+      </c>
+      <c r="C12" s="30"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="34">
+        <f>SUM(G10:G11)</f>
+        <v>61.762300164692448</v>
+      </c>
+      <c r="H12" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="34">
+        <v>64.63</v>
+      </c>
+      <c r="J12" s="9">
+        <f>G12*I12</f>
+        <v>3991.6974596440728</v>
+      </c>
       <c r="K12" s="32"/>
       <c r="M12" s="36"/>
       <c r="N12" s="1"/>
@@ -3355,28 +3464,22 @@
       <c r="R12" s="36"/>
       <c r="S12" s="36"/>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="5">
-        <v>1</v>
-      </c>
-      <c r="D13" s="8">
-        <v>1</v>
-      </c>
-      <c r="E13" s="8">
-        <v>1</v>
-      </c>
-      <c r="F13" s="8">
-        <v>1.5</v>
-      </c>
-      <c r="G13" s="63">
-        <f>C13*(PI())*(D13*E13/4)*F13</f>
-        <v>1.1780972450961724</v>
-      </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
+      <c r="B13" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="30"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="9">
+        <f>0.13*G12*19284/360</f>
+        <v>430.09207091353005</v>
+      </c>
       <c r="K13" s="32"/>
       <c r="M13" s="36"/>
       <c r="N13" s="1"/>
@@ -3386,29 +3489,17 @@
       <c r="R13" s="36"/>
       <c r="S13" s="36"/>
     </row>
-    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29"/>
-      <c r="B14" s="60" t="s">
-        <v>58</v>
-      </c>
+      <c r="B14" s="35"/>
       <c r="C14" s="30"/>
       <c r="D14" s="31"/>
       <c r="E14" s="32"/>
       <c r="F14" s="32"/>
-      <c r="G14" s="34">
-        <f>SUM(G10:G13)</f>
-        <v>20.430530633326985</v>
-      </c>
-      <c r="H14" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14" s="34">
-        <v>67.510000000000005</v>
-      </c>
-      <c r="J14" s="9">
-        <f>G14*I14</f>
-        <v>1379.265123055905</v>
-      </c>
+      <c r="G14" s="34"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="9"/>
       <c r="K14" s="32"/>
       <c r="M14" s="36"/>
       <c r="N14" s="1"/>
@@ -3418,10 +3509,12 @@
       <c r="R14" s="36"/>
       <c r="S14" s="36"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="60" t="s">
-        <v>51</v>
+    <row r="15" spans="1:19" ht="69" x14ac:dyDescent="0.3">
+      <c r="A15" s="29">
+        <v>2</v>
+      </c>
+      <c r="B15" s="41" t="s">
+        <v>80</v>
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="31"/>
@@ -3430,10 +3523,7 @@
       <c r="G15" s="34"/>
       <c r="H15" s="33"/>
       <c r="I15" s="34"/>
-      <c r="J15" s="9">
-        <f>0.13*G14*20400/360</f>
-        <v>150.50490899884213</v>
-      </c>
+      <c r="J15" s="9"/>
       <c r="K15" s="32"/>
       <c r="M15" s="36"/>
       <c r="N15" s="1"/>
@@ -3443,17 +3533,32 @@
       <c r="R15" s="36"/>
       <c r="S15" s="36"/>
     </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="29"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="9"/>
+      <c r="B16" s="60" t="str">
+        <f>B11</f>
+        <v>-Manhole</v>
+      </c>
+      <c r="C16" s="5">
+        <f>C11</f>
+        <v>5</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="E16" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="G16" s="63">
+        <f>C16*(PI())*(D16*E16/4)*F16</f>
+        <v>0.84823001646924412</v>
+      </c>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
       <c r="K16" s="32"/>
       <c r="M16" s="36"/>
       <c r="N16" s="1"/>
@@ -3463,114 +3568,111 @@
       <c r="R16" s="36"/>
       <c r="S16" s="36"/>
     </row>
-    <row r="17" spans="1:19" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
-        <v>2</v>
-      </c>
-      <c r="B17" s="58" t="s">
-        <v>59</v>
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="60" t="s">
+        <v>58</v>
       </c>
       <c r="C17" s="48"/>
       <c r="D17" s="49"/>
       <c r="E17" s="49"/>
       <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="50"/>
+      <c r="G17" s="52">
+        <f>SUM(G16:G16)</f>
+        <v>0.84823001646924412</v>
+      </c>
+      <c r="H17" s="52" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="53">
+        <v>4561.53</v>
+      </c>
+      <c r="J17" s="50">
+        <f>G17*I17</f>
+        <v>3869.226667024951</v>
+      </c>
       <c r="K17" s="5"/>
     </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
-      <c r="B18" s="60" t="str">
-        <f>B12</f>
-        <v>-Manhole</v>
-      </c>
-      <c r="C18" s="5">
-        <f>C12</f>
-        <v>3</v>
-      </c>
-      <c r="D18" s="5">
-        <f t="shared" ref="D18:E18" si="1">D12</f>
-        <v>1</v>
-      </c>
-      <c r="E18" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F18" s="8">
-        <v>0.15</v>
-      </c>
-      <c r="G18" s="63">
-        <f>C18*(PI())*(D18*E18/4)*F18</f>
-        <v>0.35342917352885173</v>
-      </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="32"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="36"/>
-      <c r="S18" s="36"/>
-    </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="48"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="55">
+        <f>0.13*G17*(15452.6/5)</f>
+        <v>340.79133796480869</v>
+      </c>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
-      <c r="B19" s="60" t="s">
-        <v>58</v>
-      </c>
+      <c r="B19" s="60"/>
       <c r="C19" s="48"/>
       <c r="D19" s="49"/>
       <c r="E19" s="49"/>
       <c r="F19" s="49"/>
-      <c r="G19" s="52">
-        <f>SUM(G18:G18)</f>
-        <v>0.35342917352885173</v>
-      </c>
-      <c r="H19" s="52" t="s">
-        <v>56</v>
-      </c>
-      <c r="I19" s="53">
-        <v>4370.5200000000004</v>
-      </c>
-      <c r="J19" s="50">
-        <f>G19*I19</f>
-        <v>1544.6692714913172</v>
-      </c>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="55"/>
       <c r="K19" s="5"/>
     </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="60" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="54"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="55">
-        <f>0.13*G19*(14817.6/5)</f>
-        <v>136.16127516370895</v>
-      </c>
-      <c r="K20" s="5"/>
-    </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="69" x14ac:dyDescent="0.3">
+      <c r="A20" s="29">
+        <v>3</v>
+      </c>
+      <c r="B20" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="32"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="36"/>
+      <c r="S20" s="36"/>
+    </row>
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="9"/>
+      <c r="B21" s="60" t="str">
+        <f>B16</f>
+        <v>-Manhole</v>
+      </c>
+      <c r="C21" s="5">
+        <v>5</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="E21" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="F21" s="61">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G21" s="63">
+        <f>C21*(PI())*(D21*E21/4)*F21</f>
+        <v>0.42411500823462206</v>
+      </c>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
       <c r="K21" s="32"/>
       <c r="M21" s="36"/>
       <c r="N21" s="1"/>
@@ -3580,243 +3682,201 @@
       <c r="R21" s="36"/>
       <c r="S21" s="36"/>
     </row>
-    <row r="22" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="29">
-        <v>3</v>
-      </c>
-      <c r="B22" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="32"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="36"/>
-      <c r="S22" s="36"/>
-    </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
-      <c r="B23" s="60" t="str">
-        <f>B18</f>
-        <v>-Manhole</v>
-      </c>
-      <c r="C23" s="61">
-        <f t="shared" ref="C23:E23" si="2">C18</f>
-        <v>3</v>
-      </c>
-      <c r="D23" s="61">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E23" s="61">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F23" s="61">
-        <v>0.1</v>
-      </c>
-      <c r="G23" s="63">
-        <f>C23*(PI())*(D23*E23/4)*F23</f>
-        <v>0.23561944901923448</v>
-      </c>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="32"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="36"/>
-      <c r="S23" s="36"/>
-    </row>
-    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
-      <c r="B24" s="60" t="s">
+    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="11"/>
+      <c r="B22" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="48"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="52">
+        <f>SUM(G21:G21)</f>
+        <v>0.42411500823462206</v>
+      </c>
+      <c r="H22" s="52" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="53">
+        <v>10634.5</v>
+      </c>
+      <c r="J22" s="50">
+        <f>G22*I22</f>
+        <v>4510.2510550710886</v>
+      </c>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11"/>
+      <c r="B23" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="48"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="55">
+        <f>0.13*G22*((114907.3+6135.3)/15)</f>
+        <v>444.91185522974729</v>
+      </c>
+      <c r="K23" s="5"/>
+    </row>
+    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="1:19" ht="69" x14ac:dyDescent="0.3">
+      <c r="A25" s="29">
+        <v>4</v>
+      </c>
+      <c r="B25" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="97" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="98" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25" s="98" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" s="34"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="32"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="36"/>
+      <c r="S25" s="36"/>
+    </row>
+    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="29"/>
+      <c r="B26" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="61">
-        <f>C23</f>
-        <v>3</v>
-      </c>
-      <c r="D24" s="61">
-        <f t="shared" ref="D24:F24" si="3">D23</f>
-        <v>1</v>
-      </c>
-      <c r="E24" s="61">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="F24" s="61">
-        <f t="shared" si="3"/>
-        <v>0.1</v>
-      </c>
-      <c r="G24" s="63">
-        <f>C24*(PI())*(D24*E24/4)*F24</f>
-        <v>0.23561944901923448</v>
-      </c>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="32"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="36"/>
-      <c r="S24" s="36"/>
-    </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="60" t="s">
+      <c r="C26" s="61">
+        <f>5*2*TRUNC(D26/0.15,0)+1</f>
+        <v>61</v>
+      </c>
+      <c r="D26" s="61">
+        <v>0.9</v>
+      </c>
+      <c r="E26" s="61">
+        <f>12*12/162</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F26" s="61">
+        <f>PRODUCT(C26:E26)</f>
+        <v>48.8</v>
+      </c>
+      <c r="G26" s="95">
+        <f>F26/1000</f>
+        <v>4.8799999999999996E-2</v>
+      </c>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="32"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="36"/>
+      <c r="S26" s="36"/>
+    </row>
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+      <c r="B27" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="48"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="52">
-        <f>SUM(G23:G24)</f>
-        <v>0.47123889803846897</v>
-      </c>
-      <c r="H25" s="52" t="s">
-        <v>56</v>
-      </c>
-      <c r="I25" s="53">
-        <v>11435.3</v>
-      </c>
-      <c r="J25" s="50">
-        <f>G25*I25</f>
-        <v>5388.7581707393038</v>
-      </c>
-      <c r="K25" s="5"/>
-    </row>
-    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="60" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="48"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="54"/>
-      <c r="J26" s="55">
-        <f>0.13*G25*((127597.3+6597.3)/15)</f>
-        <v>548.06020036484711</v>
-      </c>
-      <c r="K26" s="5"/>
-    </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="60"/>
       <c r="C27" s="48"/>
       <c r="D27" s="49"/>
       <c r="E27" s="49"/>
       <c r="F27" s="49"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="54"/>
-      <c r="J27" s="55"/>
+      <c r="G27" s="96">
+        <f>SUM(G25:G26)</f>
+        <v>4.8799999999999996E-2</v>
+      </c>
+      <c r="H27" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="I27" s="53">
+        <v>124140</v>
+      </c>
+      <c r="J27" s="50">
+        <f>G27*I27</f>
+        <v>6058.0319999999992</v>
+      </c>
       <c r="K27" s="5"/>
     </row>
-    <row r="28" spans="1:19" ht="105" x14ac:dyDescent="0.25">
-      <c r="A28" s="29">
-        <v>4</v>
-      </c>
-      <c r="B28" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="32"/>
-      <c r="M28" s="36"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="36"/>
-      <c r="S28" s="36"/>
-    </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
-      <c r="B29" s="60" t="str">
-        <f>B23</f>
-        <v>-Manhole</v>
-      </c>
-      <c r="C29" s="61">
-        <f t="shared" ref="C29" si="4">C24</f>
-        <v>3</v>
-      </c>
-      <c r="D29" s="61">
-        <f>D24-0.23</f>
-        <v>0.77</v>
-      </c>
-      <c r="E29" s="61">
-        <v>0.23</v>
-      </c>
-      <c r="F29" s="61">
-        <v>1.2</v>
-      </c>
-      <c r="G29" s="63">
-        <f>C29*(PI())*(D29)*E29*F29</f>
-        <v>2.0029538122227084</v>
-      </c>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="32"/>
-      <c r="M29" s="36"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="36"/>
-      <c r="S29" s="36"/>
-    </row>
-    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
-      <c r="B30" s="60"/>
-      <c r="C30" s="61">
-        <v>1</v>
-      </c>
-      <c r="D30" s="61">
-        <f>D24-0.23</f>
-        <v>0.77</v>
-      </c>
-      <c r="E30" s="61">
-        <v>0.23</v>
-      </c>
-      <c r="F30" s="61">
-        <v>1.5</v>
-      </c>
-      <c r="G30" s="63">
-        <f>C30*(PI())*(D30)*E30*F30</f>
-        <v>0.8345640884261285</v>
-      </c>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
+    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="11"/>
+      <c r="B28" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="48"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="55">
+        <f>0.13*G27*110960</f>
+        <v>703.93024000000003</v>
+      </c>
+      <c r="K28" s="5"/>
+    </row>
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="11"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="55"/>
+      <c r="K29" s="5"/>
+    </row>
+    <row r="30" spans="1:19" ht="69" x14ac:dyDescent="0.3">
+      <c r="A30" s="29">
+        <v>5</v>
+      </c>
+      <c r="B30" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="30"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="9"/>
       <c r="K30" s="32"/>
       <c r="M30" s="36"/>
       <c r="N30" s="1"/>
@@ -3826,27 +3886,28 @@
       <c r="R30" s="36"/>
       <c r="S30" s="36"/>
     </row>
-    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="29"/>
-      <c r="B31" s="60" t="s">
-        <v>79</v>
+      <c r="B31" s="60" t="str">
+        <f>B26</f>
+        <v>-Manhole cover</v>
       </c>
       <c r="C31" s="61">
-        <f>-2*4</f>
-        <v>-8</v>
+        <f>C16</f>
+        <v>5</v>
       </c>
       <c r="D31" s="61">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E31" s="61">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="F31" s="61">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="G31" s="63">
-        <f>C31*(PI())*(D31*F31/4)*E31</f>
-        <v>-0.52024774343446978</v>
+        <f>C31*(PI())*(D31*E31/4)*F31</f>
+        <v>0.39269908169872414</v>
       </c>
       <c r="H31" s="11"/>
       <c r="I31" s="11"/>
@@ -3860,7 +3921,7 @@
       <c r="R31" s="36"/>
       <c r="S31" s="36"/>
     </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11"/>
       <c r="B32" s="60" t="s">
         <v>58</v>
@@ -3870,22 +3931,22 @@
       <c r="E32" s="49"/>
       <c r="F32" s="49"/>
       <c r="G32" s="52">
-        <f>SUM(G29:G31)</f>
-        <v>2.317270157214367</v>
+        <f>SUM(G31:G31)</f>
+        <v>0.39269908169872414</v>
       </c>
       <c r="H32" s="52" t="s">
         <v>56</v>
       </c>
       <c r="I32" s="53">
-        <v>14197.17</v>
+        <v>11588.17</v>
       </c>
       <c r="J32" s="50">
         <f>G32*I32</f>
-        <v>32898.678357899094</v>
+        <v>4550.6637175687038</v>
       </c>
       <c r="K32" s="5"/>
     </row>
-    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
       <c r="B33" s="60" t="s">
         <v>51</v>
@@ -3898,12 +3959,12 @@
       <c r="H33" s="54"/>
       <c r="I33" s="54"/>
       <c r="J33" s="55">
-        <f>0.13*G32*((53435.9)/5)</f>
-        <v>3219.4608262411712</v>
+        <f>0.13*G32*((128662.2+6685.5)/15)</f>
+        <v>460.64128500029824</v>
       </c>
       <c r="K33" s="5"/>
     </row>
-    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11"/>
       <c r="B34" s="60"/>
       <c r="C34" s="48"/>
@@ -3916,22 +3977,21 @@
       <c r="J34" s="55"/>
       <c r="K34" s="5"/>
     </row>
-    <row r="35" spans="1:19" ht="105" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A35" s="29">
-        <v>5</v>
-      </c>
-      <c r="B35" s="41" t="str">
-        <f>description_247</f>
-        <v>Providing and Laying Reinforced cement concrete NP3 Flush jointed pipe for culverts including fixing with cement mortar 1:2 as per Drawing and Technical Specifications., 450 mm  internal dia.</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
+        <v>6</v>
+      </c>
+      <c r="B35" s="100" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="30"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="9"/>
       <c r="K35" s="32"/>
       <c r="M35" s="36"/>
       <c r="N35" s="1"/>
@@ -3941,23 +4001,28 @@
       <c r="R35" s="36"/>
       <c r="S35" s="36"/>
     </row>
-    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="29"/>
-      <c r="B36" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="C36" s="5">
-        <f>D11/2.5</f>
-        <v>20</v>
-      </c>
-      <c r="D36" s="8">
-        <v>2.5</v>
-      </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
+      <c r="B36" s="60" t="str">
+        <f>B31</f>
+        <v>-Manhole cover</v>
+      </c>
+      <c r="C36" s="61">
+        <v>5</v>
+      </c>
+      <c r="D36" s="61">
+        <f>1.2-0.23</f>
+        <v>0.97</v>
+      </c>
+      <c r="E36" s="61">
+        <v>0.23</v>
+      </c>
+      <c r="F36" s="61">
+        <v>1.5</v>
+      </c>
       <c r="G36" s="63">
-        <f>PRODUCT(C36:F36)</f>
-        <v>50</v>
+        <f>C36*(PI())*(D36)*E36*F36</f>
+        <v>5.2566699076191217</v>
       </c>
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
@@ -3971,29 +4036,31 @@
       <c r="R36" s="36"/>
       <c r="S36" s="36"/>
     </row>
-    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="29"/>
       <c r="B37" s="60" t="s">
-        <v>58</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="43">
-        <f>SUM(G36:G36)</f>
-        <v>50</v>
-      </c>
-      <c r="H37" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="I37" s="11">
-        <v>5129.82</v>
-      </c>
-      <c r="J37" s="11">
-        <f>G37*I37</f>
-        <v>256491</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C37" s="61">
+        <f>-2*5</f>
+        <v>-10</v>
+      </c>
+      <c r="D37" s="61">
+        <v>0.6</v>
+      </c>
+      <c r="E37" s="61">
+        <v>0.23</v>
+      </c>
+      <c r="F37" s="61">
+        <v>0.6</v>
+      </c>
+      <c r="G37" s="63">
+        <f>C37*(PI())*(D37*F37/4)*E37</f>
+        <v>-0.65030967929308725</v>
+      </c>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
       <c r="K37" s="32"/>
       <c r="M37" s="36"/>
       <c r="N37" s="1"/>
@@ -4003,94 +4070,75 @@
       <c r="R37" s="36"/>
       <c r="S37" s="36"/>
     </row>
-    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="29"/>
+    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="11"/>
       <c r="B38" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="48"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="52">
+        <f>SUM(G36:G37)</f>
+        <v>4.6063602283260341</v>
+      </c>
+      <c r="H38" s="52" t="s">
+        <v>56</v>
+      </c>
+      <c r="I38" s="53">
+        <v>14362.76</v>
+      </c>
+      <c r="J38" s="50">
+        <f>G38*I38</f>
+        <v>66160.046432992036</v>
+      </c>
+      <c r="K38" s="5"/>
+    </row>
+    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="11"/>
+      <c r="B39" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11">
-        <f>0.13*G37*((57525.6)/12.5)</f>
-        <v>29913.311999999998</v>
-      </c>
-      <c r="K38" s="32"/>
-      <c r="M38" s="36"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="36"/>
-      <c r="S38" s="36"/>
-    </row>
-    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="29"/>
-      <c r="B39" s="60"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="32"/>
-      <c r="M39" s="36"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="36"/>
-      <c r="S39" s="36"/>
-    </row>
-    <row r="40" spans="1:19" ht="105" x14ac:dyDescent="0.25">
-      <c r="A40" s="29">
-        <v>6</v>
-      </c>
-      <c r="B40" s="41" t="str">
-        <f>description_248</f>
-        <v>Providing and Laying Reinforced cement concrete NP3 Flush jointed pipe for culverts including fixing with cement mortar 1:2 as per Drawing and Technical Specifications., 600 mm  internal dia.</v>
-      </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="32"/>
-      <c r="M40" s="36"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="36"/>
-      <c r="S40" s="36"/>
-    </row>
-    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="29"/>
-      <c r="B41" s="60" t="s">
-        <v>76</v>
-      </c>
-      <c r="C41" s="5">
-        <f>D10/2.5</f>
-        <v>7</v>
-      </c>
-      <c r="D41" s="8">
-        <v>2.5</v>
-      </c>
+      <c r="C39" s="48"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="54"/>
+      <c r="H39" s="54"/>
+      <c r="I39" s="54"/>
+      <c r="J39" s="55">
+        <f>0.13*G38*10311.74</f>
+        <v>6174.946572709031</v>
+      </c>
+      <c r="K39" s="5"/>
+    </row>
+    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="11"/>
+      <c r="B40" s="60"/>
+      <c r="C40" s="48"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="49"/>
+      <c r="G40" s="54"/>
+      <c r="H40" s="54"/>
+      <c r="I40" s="54"/>
+      <c r="J40" s="55"/>
+      <c r="K40" s="5"/>
+    </row>
+    <row r="41" spans="1:19" ht="82.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="29">
+        <v>5</v>
+      </c>
+      <c r="B41" s="41" t="str">
+        <f>description_247</f>
+        <v>Providing and Laying Reinforced cement concrete NP3 Flush jointed pipe for culverts including fixing with cement mortar 1:2 as per Drawing and Technical Specifications., 450 mm  internal dia.</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="8"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
-      <c r="G41" s="63">
-        <f>PRODUCT(C41:F41)</f>
-        <v>17.5</v>
-      </c>
+      <c r="G41" s="9"/>
       <c r="H41" s="11"/>
       <c r="I41" s="11"/>
       <c r="J41" s="11"/>
@@ -4103,29 +4151,26 @@
       <c r="R41" s="36"/>
       <c r="S41" s="36"/>
     </row>
-    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="29"/>
       <c r="B42" s="60" t="s">
-        <v>58</v>
-      </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="8"/>
+        <v>77</v>
+      </c>
+      <c r="C42" s="5">
+        <v>0</v>
+      </c>
+      <c r="D42" s="8">
+        <v>2.5</v>
+      </c>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
-      <c r="G42" s="43">
-        <f>SUM(G41:G41)</f>
-        <v>17.5</v>
-      </c>
-      <c r="H42" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="I42" s="11">
-        <v>6915.37</v>
-      </c>
-      <c r="J42" s="11">
-        <f>G42*I42</f>
-        <v>121018.97499999999</v>
-      </c>
+      <c r="G42" s="63">
+        <f>PRODUCT(C42:F42)</f>
+        <v>0</v>
+      </c>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
       <c r="K42" s="32"/>
       <c r="M42" s="36"/>
       <c r="N42" s="1"/>
@@ -4135,21 +4180,28 @@
       <c r="R42" s="36"/>
       <c r="S42" s="36"/>
     </row>
-    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="29"/>
       <c r="B43" s="60" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
+      <c r="G43" s="43">
+        <f>SUM(G42:G42)</f>
+        <v>0</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="I43" s="11">
+        <v>5129.82</v>
+      </c>
       <c r="J43" s="11">
-        <f>0.13*G42*((78948.9)/12.5)</f>
-        <v>14368.699799999999</v>
+        <f>G43*I43</f>
+        <v>0</v>
       </c>
       <c r="K43" s="32"/>
       <c r="M43" s="36"/>
@@ -4160,9 +4212,11 @@
       <c r="R43" s="36"/>
       <c r="S43" s="36"/>
     </row>
-    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="29"/>
-      <c r="B44" s="60"/>
+      <c r="B44" s="60" t="s">
+        <v>51</v>
+      </c>
       <c r="C44" s="5"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
@@ -4170,7 +4224,10 @@
       <c r="G44" s="9"/>
       <c r="H44" s="11"/>
       <c r="I44" s="11"/>
-      <c r="J44" s="11"/>
+      <c r="J44" s="11">
+        <f>0.13*G43*((57525.6)/12.5)</f>
+        <v>0</v>
+      </c>
       <c r="K44" s="32"/>
       <c r="M44" s="36"/>
       <c r="N44" s="1"/>
@@ -4180,33 +4237,17 @@
       <c r="R44" s="36"/>
       <c r="S44" s="36"/>
     </row>
-    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="29">
-        <v>7</v>
-      </c>
-      <c r="B45" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="C45" s="30">
-        <v>1</v>
-      </c>
-      <c r="D45" s="31"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="43">
-        <f t="shared" ref="G45" si="5">PRODUCT(C45:F45)</f>
-        <v>1</v>
-      </c>
-      <c r="H45" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="I45" s="34">
-        <v>500</v>
-      </c>
-      <c r="J45" s="43">
-        <f>G45*I45</f>
-        <v>500</v>
-      </c>
+    <row r="45" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="29"/>
+      <c r="B45" s="60"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
       <c r="K45" s="32"/>
       <c r="M45" s="36"/>
       <c r="N45" s="1"/>
@@ -4216,17 +4257,21 @@
       <c r="R45" s="36"/>
       <c r="S45" s="36"/>
     </row>
-    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="29"/>
-      <c r="B46" s="35"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="34"/>
-      <c r="H46" s="33"/>
-      <c r="I46" s="34"/>
-      <c r="J46" s="9"/>
+    <row r="46" spans="1:19" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="29">
+        <v>7</v>
+      </c>
+      <c r="B46" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" s="5"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
       <c r="K46" s="32"/>
       <c r="M46" s="36"/>
       <c r="N46" s="1"/>
@@ -4236,117 +4281,283 @@
       <c r="R46" s="36"/>
       <c r="S46" s="36"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
-      <c r="B47" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C47" s="10"/>
-      <c r="D47" s="8"/>
+    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="29"/>
+      <c r="B47" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" s="5">
+        <f>(45+15)/2.5</f>
+        <v>24</v>
+      </c>
+      <c r="D47" s="8">
+        <v>2.5</v>
+      </c>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9">
-        <f>SUM(J9:J45)</f>
-        <v>467557.54493395414</v>
-      </c>
-      <c r="K47" s="5"/>
-    </row>
-    <row r="49" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="18" t="s">
+      <c r="G47" s="63">
+        <f>PRODUCT(C47:F47)</f>
+        <v>60</v>
+      </c>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="32"/>
+      <c r="M47" s="36"/>
+      <c r="N47" s="1">
+        <f>44/2.5</f>
+        <v>17.600000000000001</v>
+      </c>
+      <c r="O47" s="1">
+        <f>45/2.5</f>
+        <v>18</v>
+      </c>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="36"/>
+      <c r="S47" s="36"/>
+    </row>
+    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="29"/>
+      <c r="B48" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="43">
+        <f>SUM(G47:G47)</f>
+        <v>60</v>
+      </c>
+      <c r="H48" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="I48" s="11">
+        <v>6932.79</v>
+      </c>
+      <c r="J48" s="11">
+        <f>G48*I48</f>
+        <v>415967.4</v>
+      </c>
+      <c r="K48" s="32"/>
+      <c r="M48" s="36"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="36"/>
+      <c r="S48" s="36"/>
+    </row>
+    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="29"/>
+      <c r="B49" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11">
+        <f>0.13*G48*((78764.9)/12.5)</f>
+        <v>49149.297599999998</v>
+      </c>
+      <c r="K49" s="32"/>
+      <c r="M49" s="36"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="36"/>
+      <c r="S49" s="36"/>
+    </row>
+    <row r="50" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="29"/>
+      <c r="B50" s="60"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="32"/>
+      <c r="M50" s="36"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="36"/>
+      <c r="S50" s="36"/>
+    </row>
+    <row r="51" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="29">
+        <v>8</v>
+      </c>
+      <c r="B51" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C51" s="30">
+        <v>1</v>
+      </c>
+      <c r="D51" s="31"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="43">
+        <f t="shared" ref="G51" si="0">PRODUCT(C51:F51)</f>
+        <v>1</v>
+      </c>
+      <c r="H51" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="I51" s="34">
+        <v>500</v>
+      </c>
+      <c r="J51" s="43">
+        <f>G51*I51</f>
+        <v>500</v>
+      </c>
+      <c r="K51" s="32"/>
+      <c r="M51" s="36"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="36"/>
+      <c r="S51" s="36"/>
+    </row>
+    <row r="52" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="29"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="31"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="34"/>
+      <c r="H52" s="33"/>
+      <c r="I52" s="34"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="32"/>
+      <c r="M52" s="36"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="36"/>
+      <c r="S52" s="36"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A53" s="11"/>
+      <c r="B53" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="10"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9">
+        <f>SUM(J9:J51)</f>
+        <v>563311.92829411826</v>
+      </c>
+      <c r="K53" s="5"/>
+    </row>
+    <row r="55" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C49" s="70">
-        <f>J47</f>
-        <v>467557.54493395414</v>
-      </c>
-      <c r="D49" s="71"/>
-      <c r="E49" s="16">
+      <c r="C55" s="72">
+        <f>J53</f>
+        <v>563311.92829411826</v>
+      </c>
+      <c r="D55" s="73"/>
+      <c r="E55" s="16">
         <v>100</v>
       </c>
-      <c r="F49" s="20"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="20"/>
-      <c r="I49" s="22"/>
-      <c r="J49" s="23"/>
-      <c r="K49" s="24"/>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="18" t="s">
+      <c r="F55" s="20"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="22"/>
+      <c r="J55" s="23"/>
+      <c r="K55" s="24"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A56" s="99"/>
+      <c r="B56" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C50" s="72">
-        <v>400000</v>
-      </c>
-      <c r="D50" s="73"/>
-      <c r="E50" s="16"/>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B51" s="18" t="s">
+      <c r="C56" s="79">
+        <v>500000</v>
+      </c>
+      <c r="D56" s="80"/>
+      <c r="E56" s="16"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A57" s="99"/>
+      <c r="B57" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C51" s="72">
-        <f>C50-C53-C54</f>
-        <v>380000</v>
-      </c>
-      <c r="D51" s="73"/>
-      <c r="E51" s="16">
-        <f>C51/C49*100</f>
-        <v>81.273418452412685</v>
-      </c>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B52" s="18" t="s">
+      <c r="C57" s="79">
+        <f>C56-C59-C60</f>
+        <v>475000</v>
+      </c>
+      <c r="D57" s="80"/>
+      <c r="E57" s="16">
+        <f>C57/C55*100</f>
+        <v>84.322730647377924</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A58" s="99"/>
+      <c r="B58" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C52" s="69">
-        <f>C49-C51</f>
-        <v>87557.544933954137</v>
-      </c>
-      <c r="D52" s="69"/>
-      <c r="E52" s="16">
-        <f>100-E51</f>
-        <v>18.726581547587315</v>
-      </c>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B53" s="18" t="s">
+      <c r="C58" s="78">
+        <f>C55-C57</f>
+        <v>88311.928294118261</v>
+      </c>
+      <c r="D58" s="78"/>
+      <c r="E58" s="16">
+        <f>100-E57</f>
+        <v>15.677269352622076</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A59" s="99"/>
+      <c r="B59" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C53" s="70">
-        <f>C50*0.03</f>
-        <v>12000</v>
-      </c>
-      <c r="D53" s="71"/>
-      <c r="E53" s="16">
+      <c r="C59" s="72">
+        <f>C56*0.03</f>
+        <v>15000</v>
+      </c>
+      <c r="D59" s="73"/>
+      <c r="E59" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B54" s="18" t="s">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A60" s="99"/>
+      <c r="B60" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C54" s="70">
-        <f>C50*0.02</f>
-        <v>8000</v>
-      </c>
-      <c r="D54" s="71"/>
-      <c r="E54" s="16">
+      <c r="C60" s="72">
+        <f>C56*0.02</f>
+        <v>10000</v>
+      </c>
+      <c r="D60" s="73"/>
+      <c r="E60" s="16">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
@@ -4354,6 +4565,14 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4365,7 +4584,7 @@
 Basudev Khanal</oddFooter>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="39" max="10" man="1"/>
+    <brk id="45" max="10" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
@@ -4378,52 +4597,52 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="90" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
-    </row>
-    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="91" t="s">
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+    </row>
+    <row r="2" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A2" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="76" t="s">
         <v>2</v>
       </c>
@@ -4438,7 +4657,7 @@
       <c r="J3" s="76"/>
       <c r="K3" s="76"/>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="76" t="s">
         <v>3</v>
       </c>
@@ -4453,31 +4672,31 @@
       <c r="J4" s="76"/>
       <c r="K4" s="76"/>
     </row>
-    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="92" t="s">
+    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="92"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-    </row>
-    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="85"/>
+    </row>
+    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="88" t="e">
+      <c r="C6" s="81" t="e">
         <f>F18</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="89"/>
+      <c r="D6" s="82"/>
       <c r="E6" s="13"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4485,90 +4704,90 @@
         <v>20</v>
       </c>
       <c r="I6" s="12"/>
-      <c r="J6" s="88">
+      <c r="J6" s="81">
         <f>I18</f>
         <v>291284.22700000001</v>
       </c>
-      <c r="K6" s="89"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6" s="82"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="I7" s="84" t="s">
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="I7" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="84"/>
-      <c r="K7" s="84"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="78" t="str">
+      <c r="J7" s="89"/>
+      <c r="K7" s="89"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="69" t="str">
         <f>Estimate!A6</f>
         <v>Project:- बेन्डोल हाईट सडक निर्माण</v>
       </c>
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="I8" s="85" t="s">
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="I8" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="J8" s="85"/>
-      <c r="K8" s="85"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="86" t="str">
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="91" t="str">
         <f>Estimate!A7</f>
         <v>Location:- Shankharapur Municipality 9</v>
       </c>
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="I9" s="85" t="s">
+      <c r="B9" s="91"/>
+      <c r="C9" s="91"/>
+      <c r="D9" s="91"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="91"/>
+      <c r="I9" s="90" t="s">
         <v>49</v>
       </c>
-      <c r="J9" s="85"/>
-      <c r="K9" s="85"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="81" t="s">
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="81" t="s">
+      <c r="C11" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="87" t="s">
+      <c r="D11" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="87"/>
-      <c r="F11" s="87"/>
-      <c r="G11" s="87" t="s">
+      <c r="E11" s="92"/>
+      <c r="F11" s="92"/>
+      <c r="G11" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="87"/>
-      <c r="I11" s="87"/>
-      <c r="J11" s="81" t="s">
+      <c r="H11" s="92"/>
+      <c r="I11" s="92"/>
+      <c r="J11" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="82" t="s">
+      <c r="K11" s="87" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="81"/>
-      <c r="B12" s="81"/>
-      <c r="C12" s="81"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="86"/>
+      <c r="B12" s="86"/>
+      <c r="C12" s="86"/>
       <c r="D12" s="15" t="s">
         <v>26</v>
       </c>
@@ -4587,10 +4806,10 @@
       <c r="I12" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="81"/>
-      <c r="K12" s="82"/>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="J12" s="86"/>
+      <c r="K12" s="87"/>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A13" s="38">
         <f>Estimate!A9</f>
         <v>1</v>
@@ -4633,7 +4852,7 @@
       </c>
       <c r="K13" s="19"/>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="38"/>
       <c r="B14" s="45" t="e">
         <f>Estimate!#REF!</f>
@@ -4655,7 +4874,7 @@
       <c r="J14" s="39"/>
       <c r="K14" s="19"/>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="40"/>
       <c r="B15" s="40"/>
       <c r="C15" s="16"/>
@@ -4668,7 +4887,7 @@
       <c r="J15" s="39"/>
       <c r="K15" s="19"/>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="38">
         <f>Estimate!A69</f>
         <v>9</v>
@@ -4711,7 +4930,7 @@
       </c>
       <c r="K16" s="19"/>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="40"/>
       <c r="B17" s="40"/>
       <c r="C17" s="16"/>
@@ -4724,7 +4943,7 @@
       <c r="J17" s="39"/>
       <c r="K17" s="19"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>16</v>
@@ -4750,13 +4969,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -4770,6 +4982,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4791,26 +5010,26 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" customWidth="1"/>
+    <col min="14" max="14" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" customWidth="1"/>
+    <col min="17" max="17" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
@@ -4825,7 +5044,7 @@
       <c r="J1" s="74"/>
       <c r="K1" s="74"/>
     </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A2" s="75" t="s">
         <v>1</v>
       </c>
@@ -4840,7 +5059,7 @@
       <c r="J2" s="75"/>
       <c r="K2" s="75"/>
     </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="76" t="s">
         <v>2</v>
       </c>
@@ -4855,7 +5074,7 @@
       <c r="J3" s="76"/>
       <c r="K3" s="76"/>
     </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="76" t="s">
         <v>3</v>
       </c>
@@ -4870,7 +5089,7 @@
       <c r="J4" s="76"/>
       <c r="K4" s="76"/>
     </row>
-    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="77" t="s">
         <v>31</v>
       </c>
@@ -4885,42 +5104,42 @@
       <c r="J5" s="77"/>
       <c r="K5" s="77"/>
     </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="78" t="str">
+    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="69" t="str">
         <f>Estimate!A6</f>
         <v>Project:- बेन्डोल हाईट सडक निर्माण</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="79" t="s">
+      <c r="H6" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="80" t="s">
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="79" t="s">
+      <c r="H7" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -4955,7 +5174,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="249.6" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>1</v>
       </c>
@@ -4994,7 +5213,7 @@
       <c r="R9" s="36"/>
       <c r="S9" s="36"/>
     </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29"/>
       <c r="B10" s="35"/>
       <c r="C10" s="30"/>
@@ -5024,7 +5243,7 @@
       <c r="R10" s="36"/>
       <c r="S10" s="36"/>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29"/>
       <c r="B11" s="35" t="s">
         <v>39</v>
@@ -5049,7 +5268,7 @@
       <c r="R11" s="36"/>
       <c r="S11" s="36"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29"/>
       <c r="B12" s="35"/>
       <c r="C12" s="30"/>
@@ -5069,7 +5288,7 @@
       <c r="R12" s="36"/>
       <c r="S12" s="36"/>
     </row>
-    <row r="13" spans="1:19" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A13" s="29">
         <v>2</v>
       </c>
@@ -5104,7 +5323,7 @@
       <c r="R13" s="36"/>
       <c r="S13" s="36"/>
     </row>
-    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29"/>
       <c r="B14" s="35"/>
       <c r="C14" s="30"/>
@@ -5124,7 +5343,7 @@
       <c r="R14" s="36"/>
       <c r="S14" s="36"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="28" t="s">
         <v>17</v>
@@ -5142,15 +5361,15 @@
       </c>
       <c r="K15" s="5"/>
     </row>
-    <row r="17" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="70">
+      <c r="C17" s="72">
         <f>J15</f>
         <v>291284.22700000001</v>
       </c>
-      <c r="D17" s="71"/>
+      <c r="D17" s="73"/>
       <c r="E17" s="16">
         <v>100</v>
       </c>
@@ -5161,87 +5380,87 @@
       <c r="J17" s="23"/>
       <c r="K17" s="24"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="72">
+      <c r="C18" s="79">
         <v>250000</v>
       </c>
-      <c r="D18" s="73"/>
+      <c r="D18" s="80"/>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="72">
+      <c r="C19" s="79">
         <f>C18-C21-C22</f>
         <v>237500</v>
       </c>
-      <c r="D19" s="73"/>
+      <c r="D19" s="80"/>
       <c r="E19" s="16">
         <f>C19/C17*100</f>
         <v>81.535482523741322</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="69">
+      <c r="C20" s="78">
         <f>C17-C19</f>
         <v>53784.227000000014</v>
       </c>
-      <c r="D20" s="69"/>
+      <c r="D20" s="78"/>
       <c r="E20" s="16">
         <f>100-E19</f>
         <v>18.464517476258678</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="70">
+      <c r="C21" s="72">
         <f>C18*0.03</f>
         <v>7500</v>
       </c>
-      <c r="D21" s="71"/>
+      <c r="D21" s="73"/>
       <c r="E21" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="70">
+      <c r="C22" s="72">
         <f>C18*0.02</f>
         <v>5000</v>
       </c>
-      <c r="D22" s="71"/>
+      <c r="D22" s="73"/>
       <c r="E22" s="16">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5260,26 +5479,26 @@
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="7" customWidth="1"/>
     <col min="8" max="8" width="5" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" style="7" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" style="7" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.33203125" style="7" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" style="7" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" customWidth="1"/>
+    <col min="14" max="14" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" customWidth="1"/>
+    <col min="17" max="17" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
@@ -5294,7 +5513,7 @@
       <c r="J1" s="74"/>
       <c r="K1" s="74"/>
     </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A2" s="75" t="s">
         <v>1</v>
       </c>
@@ -5309,7 +5528,7 @@
       <c r="J2" s="75"/>
       <c r="K2" s="75"/>
     </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="76" t="s">
         <v>2</v>
       </c>
@@ -5324,7 +5543,7 @@
       <c r="J3" s="76"/>
       <c r="K3" s="76"/>
     </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="76" t="s">
         <v>3</v>
       </c>
@@ -5339,7 +5558,7 @@
       <c r="J4" s="76"/>
       <c r="K4" s="76"/>
     </row>
-    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="77" t="s">
         <v>35</v>
       </c>
@@ -5354,16 +5573,16 @@
       <c r="J5" s="77"/>
       <c r="K5" s="77"/>
     </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="78" t="str">
+    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="69" t="str">
         <f>Estimate!A6</f>
         <v>Project:- बेन्डोल हाईट सडक निर्माण</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
       <c r="G6" s="94" t="s">
         <v>34</v>
       </c>
@@ -5372,15 +5591,15 @@
       <c r="J6" s="94"/>
       <c r="K6" s="94"/>
     </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="80" t="s">
+    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
       <c r="G7" s="93" t="s">
         <v>47</v>
       </c>
@@ -5389,7 +5608,7 @@
       <c r="J7" s="93"/>
       <c r="K7" s="93"/>
     </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -5424,7 +5643,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="249.6" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>1</v>
       </c>
@@ -5463,7 +5682,7 @@
       <c r="R9" s="36"/>
       <c r="S9" s="36"/>
     </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29"/>
       <c r="B10" s="35"/>
       <c r="C10" s="30"/>
@@ -5493,7 +5712,7 @@
       <c r="R10" s="36"/>
       <c r="S10" s="36"/>
     </row>
-    <row r="11" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29"/>
       <c r="B11" s="35" t="s">
         <v>39</v>
@@ -5518,7 +5737,7 @@
       <c r="R11" s="36"/>
       <c r="S11" s="36"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29"/>
       <c r="B12" s="35"/>
       <c r="C12" s="30"/>
@@ -5538,7 +5757,7 @@
       <c r="R12" s="36"/>
       <c r="S12" s="36"/>
     </row>
-    <row r="13" spans="1:19" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A13" s="29">
         <v>2</v>
       </c>
@@ -5573,7 +5792,7 @@
       <c r="R13" s="36"/>
       <c r="S13" s="36"/>
     </row>
-    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29"/>
       <c r="B14" s="35"/>
       <c r="C14" s="30"/>
@@ -5593,7 +5812,7 @@
       <c r="R14" s="36"/>
       <c r="S14" s="36"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="28" t="s">
         <v>17</v>
@@ -5611,15 +5830,15 @@
       </c>
       <c r="K15" s="5"/>
     </row>
-    <row r="17" spans="2:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="B17" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="70">
+      <c r="C17" s="72">
         <f>J15</f>
         <v>291284.22700000001</v>
       </c>
-      <c r="D17" s="71"/>
+      <c r="D17" s="73"/>
       <c r="E17" s="16">
         <v>100</v>
       </c>
@@ -5630,72 +5849,79 @@
       <c r="J17" s="23"/>
       <c r="K17" s="24"/>
     </row>
-    <row r="18" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="B18" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="72">
+      <c r="C18" s="79">
         <v>600000</v>
       </c>
-      <c r="D18" s="73"/>
+      <c r="D18" s="80"/>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="B19" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="72">
+      <c r="C19" s="79">
         <f>C18-C21-C22</f>
         <v>570000</v>
       </c>
-      <c r="D19" s="73"/>
+      <c r="D19" s="80"/>
       <c r="E19" s="16">
         <f>C19/C17*100</f>
         <v>195.68515805697916</v>
       </c>
     </row>
-    <row r="20" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="B20" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="69">
+      <c r="C20" s="78">
         <f>C17-C19</f>
         <v>-278715.77299999999</v>
       </c>
-      <c r="D20" s="69"/>
+      <c r="D20" s="78"/>
       <c r="E20" s="16">
         <f>100-E19</f>
         <v>-95.685158056979162</v>
       </c>
     </row>
-    <row r="21" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="B21" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="70">
+      <c r="C21" s="72">
         <f>C18*0.03</f>
         <v>18000</v>
       </c>
-      <c r="D21" s="71"/>
+      <c r="D21" s="73"/>
       <c r="E21" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="B22" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="70">
+      <c r="C22" s="72">
         <f>C18*0.02</f>
         <v>12000</v>
       </c>
-      <c r="D22" s="71"/>
+      <c r="D22" s="73"/>
       <c r="E22" s="16">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
     <mergeCell ref="G7:K7"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A1:K1"/>
@@ -5704,13 +5930,6 @@
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="G6:K6"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>